<commit_message>
bump schema version to 0.2.0 and new artefacts
</commit_message>
<xml_diff>
--- a/project/excel/miiid_schema.xlsx
+++ b/project/excel/miiid_schema.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,31 +472,54 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>sequence_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>evidence_type</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>method_type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
         <is>
           <t>reference</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>participant_outcomes</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"simulation,microscopy,cultivation,sample"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"not_affected,positively,negatively,not_applicable"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>